<commit_message>
SE ANEXA MODIFICACION AL MER, DIAGRAMA DE CLASES Y SE ACTUALIZA FORMATO DE SEGUIMIENTO
</commit_message>
<xml_diff>
--- a/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
+++ b/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrandonMedina/Documents/ACADEMICO/MISION TIC/DESARROLLO DE SOFTWARE/MINTIC-84-02/PROGRESO GENERAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{132B20B5-1F08-F64D-94BE-3CCCA2E262A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EC609A-9753-1345-99FF-FFC303574437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{DE7C8E90-1280-BC4D-978F-3D5EB08E9B99}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="PROGRESO GENERAL" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -90,9 +89,6 @@
   </si>
   <si>
     <t>DIAGRAMA DE CLASES: Clases, Atributos, Métodos, Asociación entre clases (Generalización, Agregación, Composición)</t>
-  </si>
-  <si>
-    <t>POSPUESTO</t>
   </si>
   <si>
     <t>Script SQL con el DDL de la Base de Datos</t>
@@ -301,7 +297,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -332,37 +358,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <right style="thin">
           <color theme="4"/>
@@ -473,12 +468,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94A0D31E-D68B-0E43-8B45-BB47CF157E6E}" name="Actividades" displayName="Actividades" ref="A1:C12" totalsRowShown="0" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94A0D31E-D68B-0E43-8B45-BB47CF157E6E}" name="Actividades" displayName="Actividades" ref="A1:C12" totalsRowShown="0" tableBorderDxfId="3">
   <autoFilter ref="A1:C12" xr:uid="{7C84295C-F6B8-8E49-B603-80146D0EE461}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2B048E4B-1680-EC48-B8DE-D898EA5342EB}" name="SPRINT"/>
+    <tableColumn id="1" xr3:uid="{2B048E4B-1680-EC48-B8DE-D898EA5342EB}" name="SPRINT" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{29528C23-2FE1-B944-8E64-F080BF8FFF23}" name="ACTIVIDAD" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{0CFA4718-6267-AE49-8125-8D496B84385B}" name="ESTADO" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{0CFA4718-6267-AE49-8125-8D496B84385B}" name="ESTADO" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -784,7 +779,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -799,7 +794,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
@@ -809,6 +804,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
       <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
@@ -817,6 +815,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
       <c r="B3" s="14" t="s">
         <v>4</v>
       </c>
@@ -825,6 +826,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
@@ -833,6 +837,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
       <c r="B5" s="14" t="s">
         <v>6</v>
       </c>
@@ -841,6 +848,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
       <c r="B6" s="14" t="s">
         <v>7</v>
       </c>
@@ -850,6 +860,9 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
@@ -858,43 +871,58 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
       <c r="B8" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>2</v>
+      </c>
       <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="11" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>2</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="11" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="C12" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -938,7 +966,7 @@
       </c>
       <c r="C20" s="4">
         <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$12,"HECHO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
@@ -947,7 +975,7 @@
       </c>
       <c r="C21" s="4">
         <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$12,"POSPUESTO")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
@@ -957,33 +985,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C12">
-    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="9" stopIfTrue="1">
       <formula>($C2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
       <formula>($C2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>($C2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>($C2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C12">
-    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>($C8="POSPUESTO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>($C8="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
       <formula>($C8="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>($C8="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>($C8="HACER")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
SE ANEXA CARPETA CON SOLUCION Y CAPAS CREADAS DEL PROYECTO
</commit_message>
<xml_diff>
--- a/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
+++ b/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrandonMedina/Documents/ACADEMICO/MISION TIC/DESARROLLO DE SOFTWARE/MINTIC-84-02/PROGRESO GENERAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EC609A-9753-1345-99FF-FFC303574437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72768670-2608-F240-AF45-535F66DA6BB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{DE7C8E90-1280-BC4D-978F-3D5EB08E9B99}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -85,9 +85,6 @@
     <t>DISEÑO: Modelo Entidad Relación (M.E.R.): Tablas, Campos, Tipo Datos, Llaves Primarias, Llaves Foráneas, Relaciones</t>
   </si>
   <si>
-    <t>VERIFICAR</t>
-  </si>
-  <si>
     <t>DIAGRAMA DE CLASES: Clases, Atributos, Métodos, Asociación entre clases (Generalización, Agregación, Composición)</t>
   </si>
   <si>
@@ -107,6 +104,27 @@
   </si>
   <si>
     <t>SPRINT</t>
+  </si>
+  <si>
+    <t>POSPUESTO</t>
+  </si>
+  <si>
+    <t>Creación Solución</t>
+  </si>
+  <si>
+    <t>Capa de Dominio</t>
+  </si>
+  <si>
+    <t>Capa de Datos</t>
+  </si>
+  <si>
+    <t>Capa de Persistencia</t>
+  </si>
+  <si>
+    <t>Capa de Presentación</t>
+  </si>
+  <si>
+    <t>Frontend - Formularios x Entidad</t>
   </si>
 </sst>
 </file>
@@ -260,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -293,40 +311,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color theme="0"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -358,101 +442,41 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <right style="thin">
           <color theme="4"/>
         </right>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -468,12 +492,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94A0D31E-D68B-0E43-8B45-BB47CF157E6E}" name="Actividades" displayName="Actividades" ref="A1:C12" totalsRowShown="0" tableBorderDxfId="3">
-  <autoFilter ref="A1:C12" xr:uid="{7C84295C-F6B8-8E49-B603-80146D0EE461}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94A0D31E-D68B-0E43-8B45-BB47CF157E6E}" name="Actividades" displayName="Actividades" ref="A1:C18" totalsRowShown="0" tableBorderDxfId="12">
+  <autoFilter ref="A1:C18" xr:uid="{7C84295C-F6B8-8E49-B603-80146D0EE461}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2B048E4B-1680-EC48-B8DE-D898EA5342EB}" name="SPRINT" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{29528C23-2FE1-B944-8E64-F080BF8FFF23}" name="ACTIVIDAD" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{0CFA4718-6267-AE49-8125-8D496B84385B}" name="ESTADO" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2B048E4B-1680-EC48-B8DE-D898EA5342EB}" name="SPRINT" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{29528C23-2FE1-B944-8E64-F080BF8FFF23}" name="ACTIVIDAD" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{0CFA4718-6267-AE49-8125-8D496B84385B}" name="ESTADO" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -776,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EBB0DA-65E8-1B46-BB9E-0B666CE58B08}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -794,7 +818,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
@@ -886,10 +910,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -897,10 +921,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -908,10 +932,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -919,104 +943,158 @@
         <v>2</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="9">
+        <v>3</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+      <c r="A14" s="9">
+        <v>3</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>3</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>3</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>3</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>3</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$12,"HACER")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="5" t="s">
+      <c r="C23" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HACER")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$12,"HACIENDO")</f>
+      <c r="C24" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HACIENDO")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$12,"VERIFICAR")</f>
+      <c r="C25" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"VERIFICAR")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HECHO")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"POSPUESTO")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$12,"HECHO")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$12,"POSPUESTO")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C12">
-    <cfRule type="expression" dxfId="12" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="C2:C18">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>($C2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>($C2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="11" stopIfTrue="1">
       <formula>($C2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
       <formula>($C2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C12">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="C8:C18">
+    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
       <formula>($C8="POSPUESTO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>($C8="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>($C8="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>($C8="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
       <formula>($C8="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C12" xr:uid="{EA767C87-0690-5447-BB5A-5B9509B3CB57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C18" xr:uid="{EA767C87-0690-5447-BB5A-5B9509B3CB57}">
       <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
SE ANEXA SCRIPT DE LA BASE DE DATOS DEL PROYECTO
</commit_message>
<xml_diff>
--- a/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
+++ b/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrandonMedina/Documents/ACADEMICO/MISION TIC/DESARROLLO DE SOFTWARE/MINTIC-84-02/PROGRESO GENERAL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRANDON\ACADEMICO\MISION TIC\CICLO 3\DESARROLLO DE SOFTWARE\MINTIC-84-02\PROGRESO GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72768670-2608-F240-AF45-535F66DA6BB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{DE7C8E90-1280-BC4D-978F-3D5EB08E9B99}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14175"/>
   </bookViews>
   <sheets>
     <sheet name="PROGRESO GENERAL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -130,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,93 +323,31 @@
   <dxfs count="13">
     <dxf>
       <font>
-        <color theme="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -426,36 +363,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -477,6 +384,96 @@
           <color theme="4"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -492,12 +489,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94A0D31E-D68B-0E43-8B45-BB47CF157E6E}" name="Actividades" displayName="Actividades" ref="A1:C18" totalsRowShown="0" tableBorderDxfId="12">
-  <autoFilter ref="A1:C18" xr:uid="{7C84295C-F6B8-8E49-B603-80146D0EE461}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Actividades" displayName="Actividades" ref="A1:C18" totalsRowShown="0" tableBorderDxfId="3">
+  <autoFilter ref="A1:C18"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2B048E4B-1680-EC48-B8DE-D898EA5342EB}" name="SPRINT" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{29528C23-2FE1-B944-8E64-F080BF8FFF23}" name="ACTIVIDAD" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{0CFA4718-6267-AE49-8125-8D496B84385B}" name="ESTADO" dataDxfId="9"/>
+    <tableColumn id="1" name="SPRINT" dataDxfId="2"/>
+    <tableColumn id="2" name="ACTIVIDAD" dataDxfId="1"/>
+    <tableColumn id="3" name="ESTADO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -799,24 +796,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EBB0DA-65E8-1B46-BB9E-0B666CE58B08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="91.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="102.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -827,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -838,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -849,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -860,7 +857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1</v>
       </c>
@@ -871,7 +868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -883,7 +880,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>1</v>
       </c>
@@ -894,7 +891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -905,7 +902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>2</v>
       </c>
@@ -916,7 +913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>2</v>
       </c>
@@ -927,7 +924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>2</v>
       </c>
@@ -935,10 +932,10 @@
         <v>18</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>2</v>
       </c>
@@ -949,69 +946,81 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>3</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>3</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>3</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="16"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>3</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="16"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>3</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="16"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>3</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1020,16 +1029,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="4">
         <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HACIENDO")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>11</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>12</v>
       </c>
@@ -1047,7 +1056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>13</v>
       </c>
@@ -1056,45 +1065,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C18">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="9" stopIfTrue="1">
       <formula>($C2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
       <formula>($C2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>($C2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>($C2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C18">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>($C8="POSPUESTO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>($C8="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
       <formula>($C8="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>($C8="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>($C8="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C18" xr:uid="{EA767C87-0690-5447-BB5A-5B9509B3CB57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C18">
       <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
SE ANEXA ACTUALIZACION DEL PROGRESO DEL SPRINT 2 Y 3, SE ANEXA TAMBIEN DISTRIBUCION DEL SPRINT 4
</commit_message>
<xml_diff>
--- a/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
+++ b/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +921,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,8 +964,8 @@
       <c r="B14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>17</v>
+      <c r="C14" s="11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -975,8 +975,8 @@
       <c r="B15" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>17</v>
+      <c r="C15" s="11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -986,8 +986,8 @@
       <c r="B16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>17</v>
+      <c r="C16" s="11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -997,8 +997,8 @@
       <c r="B17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>17</v>
+      <c r="C17" s="11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="C24" s="4">
         <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HACIENDO")</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C26" s="4">
         <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HECHO")</f>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
SE ANEXA FRONT-END DEL HOME DEL PROYECTO
</commit_message>
<xml_diff>
--- a/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
+++ b/PROGRESO GENERAL/FORMATO SEGUIMIENTO GENERAL SPRINTS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Frontend - Historias de Usuario</t>
   </si>
   <si>
-    <t>HACER</t>
-  </si>
-  <si>
     <t>Backend - Historias de Usuario</t>
   </si>
   <si>
@@ -124,13 +121,34 @@
   </si>
   <si>
     <t>Frontend - Formularios x Entidad</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Remision (Insetar-Editar-Eliminar-Consultar-Listar)</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Proveedor (Insetar-Editar-Eliminar-Consultar-Listar)</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Llantas (Insetar-Editar-Eliminar-Consultar-Listar)</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Orden de Trabajo (Insetar-Editar-Eliminar-Consultar-Listar)</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Conductor (Insetar-Editar-Eliminar-Consultar-Listar)</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Prestador (Insetar-Editar-Eliminar-Consultar-Listar)</t>
+  </si>
+  <si>
+    <t>Desarrollo Modulo Equipo (Insetar-Editar-Eliminar-Consultar-Listar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +177,12 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -277,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -315,6 +339,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,8 +519,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Actividades" displayName="Actividades" ref="A1:C18" totalsRowShown="0" tableBorderDxfId="3">
-  <autoFilter ref="A1:C18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Actividades" displayName="Actividades" ref="A1:C25" totalsRowShown="0" tableBorderDxfId="3">
+  <autoFilter ref="A1:C25"/>
   <tableColumns count="3">
     <tableColumn id="1" name="SPRINT" dataDxfId="2"/>
     <tableColumn id="2" name="ACTIVIDAD" dataDxfId="1"/>
@@ -797,15 +827,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="102.42578125" customWidth="1"/>
+    <col min="2" max="2" width="118.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" customWidth="1"/>
@@ -815,7 +845,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
@@ -940,10 +970,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>3</v>
@@ -962,7 +992,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>3</v>
@@ -973,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>3</v>
@@ -984,94 +1014,171 @@
         <v>3</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>3</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>3</v>
-      </c>
-      <c r="B17" s="17" t="s">
+      <c r="C17" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>3</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>3</v>
-      </c>
-      <c r="B18" s="17" t="s">
+      <c r="C18" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>4</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="C19" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>4</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>4</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>4</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
+        <v>4</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>4</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="19">
+        <v>4</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HACER")</f>
+      <c r="C30" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$25,"HACER")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$25,"HACIENDO")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$25,"VERIFICAR")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$25,"HECHO")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="4">
+        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$25,"POSPUESTO")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HACIENDO")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"VERIFICAR")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"HECHO")</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="4">
-        <f>COUNTIF('PROGRESO GENERAL'!$C$2:$C$18,"POSPUESTO")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C18">
+  <conditionalFormatting sqref="C2:C25">
     <cfRule type="expression" dxfId="12" priority="9" stopIfTrue="1">
       <formula>($C2="VERIFICAR")</formula>
     </cfRule>
@@ -1085,7 +1192,7 @@
       <formula>($C2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C18">
+  <conditionalFormatting sqref="C8:C25">
     <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>($C8="POSPUESTO")</formula>
     </cfRule>
@@ -1103,7 +1210,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C25">
       <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>